<commit_message>
:hammer: trigger de bitacoras terminados
</commit_message>
<xml_diff>
--- a/documents/scripts-base-datos/Tablas con bitacoras hechas.xlsx
+++ b/documents/scripts-base-datos/Tablas con bitacoras hechas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\proyecto-poa-pacc\documents\scripts-base-datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8223A8A2-0165-4DB3-8641-3EF02B04DD52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276DAF19-5AE1-4B6C-A461-5CE42C8B5792}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A72BED2B-DBF2-41B4-91C8-5172F343DEA1}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Tablas</t>
   </si>
   <si>
-    <t>Cheq</t>
-  </si>
-  <si>
     <t>Actividad</t>
   </si>
   <si>
@@ -142,6 +139,12 @@
   </si>
   <si>
     <t>usuario</t>
+  </si>
+  <si>
+    <t>Implementado al api</t>
+  </si>
+  <si>
+    <t>trigger hecho</t>
   </si>
 </sst>
 </file>
@@ -164,7 +167,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,8 +186,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -215,7 +224,7 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color theme="0"/>
       </top>
       <bottom style="thin">
         <color theme="0"/>
@@ -227,6 +236,75 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -236,30 +314,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
+        <color theme="0"/>
       </right>
       <top style="thin">
         <color theme="0"/>
       </top>
       <bottom style="thin">
-        <color theme="0"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -267,18 +356,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,283 +692,286 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5925852-6AE3-4033-AE75-4C98FC609D06}">
   <dimension ref="C2:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="36.109375" customWidth="1"/>
     <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="E2" s="2" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D5" s="15"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="D6" s="7"/>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="D10" s="3"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="D12" s="9"/>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="D23" s="9"/>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="7"/>
+        <v>22</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="12"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="8"/>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="4"/>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="D31" s="16"/>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="10"/>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C36" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C37" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="D37" s="9"/>
+      <c r="E37" s="10"/>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="10"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C39" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="D39" s="14"/>
+      <c r="E39" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>